<commit_message>
interface with new sim grid
</commit_message>
<xml_diff>
--- a/in/2cam_transverse.xlsx
+++ b/in/2cam_transverse.xlsx
@@ -162,6 +162,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="H11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Put Z at end for UTC—required!</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -280,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="141">
   <si>
     <t>Sim</t>
   </si>
@@ -345,6 +358,9 @@
     <t>TranscarDataDir</t>
   </si>
   <si>
+    <t>~/U/transcar/out/gfortran</t>
+  </si>
+  <si>
     <t>ExcitationDATfn</t>
   </si>
   <si>
@@ -354,9 +370,15 @@
     <t>tReq</t>
   </si>
   <si>
+    <t>2013-03-31T09:00:30Z</t>
+  </si>
+  <si>
     <t>simconfig</t>
   </si>
   <si>
+    <t>DATCAR</t>
+  </si>
+  <si>
     <t>useActualData</t>
   </si>
   <si>
@@ -366,7 +388,7 @@
     <t>BeamEnergyFN</t>
   </si>
   <si>
-    <t>~/transcar/2014-04branch/dir.transcar.server/BT_E1E2prev.csv</t>
+    <t>../transcar/dir.transcar.server/BT_E1E2prev.csv</t>
   </si>
   <si>
     <t>reactionParam</t>
@@ -378,7 +400,7 @@
     <t>altitudePreload</t>
   </si>
   <si>
-    <t>../transcar-utils/precompute/zTranscar.h5</t>
+    <t>../transcar/dir.transcar.server/dir.input/conttanh.dat</t>
   </si>
   <si>
     <t>downsampleEnergy</t>
@@ -706,7 +728,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0.00E+000"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -759,6 +781,14 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Sans"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -994,7 +1024,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1039,11 +1069,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1051,7 +1089,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1059,7 +1097,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1067,11 +1105,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1083,7 +1125,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1159,19 +1201,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1195,7 +1237,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1312,9 +1354,9 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+      <selection pane="bottomLeft" activeCell="D46" activeCellId="0" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1428,47 +1470,53 @@
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="13"/>
       <c r="G9" s="0"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="0"/>
-      <c r="C10" s="11"/>
+      <c r="C10" s="13"/>
       <c r="G10" s="0"/>
-      <c r="H10" s="11" t="s">
-        <v>22</v>
+      <c r="H10" s="14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="5"/>
       <c r="G11" s="0"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="5"/>
       <c r="G12" s="0"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0</v>
@@ -1477,9 +1525,9 @@
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0"/>
       <c r="C14" s="7"/>
@@ -1488,44 +1536,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0"/>
       <c r="C15" s="7"/>
       <c r="G15" s="0"/>
-      <c r="H15" s="14" t="s">
-        <v>28</v>
+      <c r="H15" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="7"/>
       <c r="G16" s="0"/>
-      <c r="H16" s="14" t="s">
-        <v>30</v>
+      <c r="H16" s="16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="7"/>
       <c r="G17" s="0"/>
-      <c r="H17" s="14" t="s">
-        <v>32</v>
+      <c r="H17" s="16" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="16"/>
+      <c r="A18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="18"/>
       <c r="C18" s="7"/>
       <c r="G18" s="0"/>
       <c r="H18" s="1" t="n">
@@ -1539,96 +1587,108 @@
       <c r="H19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="18"/>
+      <c r="A20" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="20"/>
       <c r="C20" s="7"/>
       <c r="G20" s="0"/>
       <c r="H20" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="19"/>
+        <v>39</v>
+      </c>
+      <c r="B21" s="21"/>
       <c r="C21" s="7"/>
       <c r="G21" s="0"/>
-      <c r="H21" s="0"/>
+      <c r="H21" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="B22" s="21"/>
       <c r="C22" s="7"/>
       <c r="G22" s="0"/>
-      <c r="H22" s="0"/>
+      <c r="H22" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="19"/>
+        <v>41</v>
+      </c>
+      <c r="B23" s="21"/>
       <c r="C23" s="7"/>
       <c r="G23" s="0"/>
-      <c r="H23" s="0"/>
+      <c r="H23" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="19"/>
+        <v>42</v>
+      </c>
+      <c r="B24" s="21"/>
       <c r="C24" s="7"/>
       <c r="G24" s="0"/>
-      <c r="H24" s="0"/>
+      <c r="H24" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="19"/>
+        <v>43</v>
+      </c>
+      <c r="B25" s="21"/>
       <c r="C25" s="7"/>
       <c r="G25" s="0"/>
-      <c r="H25" s="0"/>
+      <c r="H25" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="19"/>
+        <v>44</v>
+      </c>
+      <c r="B26" s="21"/>
       <c r="C26" s="7"/>
       <c r="G26" s="0"/>
-      <c r="H26" s="0"/>
+      <c r="H26" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
-      <c r="B27" s="19"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="7"/>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="19"/>
+        <v>45</v>
+      </c>
+      <c r="B28" s="21"/>
       <c r="C28" s="7"/>
       <c r="G28" s="0"/>
-      <c r="H28" s="12" t="n">
+      <c r="H28" s="22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="G29" s="0"/>
-      <c r="H29" s="20"/>
+      <c r="H29" s="23"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
@@ -1638,24 +1698,24 @@
       <c r="H30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="22" t="n">
+      <c r="A31" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="C31" s="22"/>
+      <c r="C31" s="25"/>
       <c r="G31" s="0"/>
       <c r="H31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="19" t="n">
+      <c r="A32" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="C32" s="19"/>
+      <c r="C32" s="21"/>
       <c r="G32" s="0"/>
       <c r="H32" s="0"/>
     </row>
@@ -1667,13 +1727,13 @@
       <c r="H33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="23" t="s">
-        <v>46</v>
+      <c r="A34" s="26" t="s">
+        <v>49</v>
       </c>
       <c r="B34" s="0"/>
       <c r="C34" s="0"/>
-      <c r="G34" s="24" t="s">
-        <v>47</v>
+      <c r="G34" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="H34" s="0"/>
     </row>
@@ -1685,121 +1745,119 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B36" s="0"/>
       <c r="C36" s="0"/>
-      <c r="G36" s="25"/>
+      <c r="G36" s="28"/>
       <c r="H36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B37" s="0"/>
       <c r="C37" s="0"/>
-      <c r="G37" s="26"/>
+      <c r="G37" s="29"/>
       <c r="H37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
       <c r="B38" s="0"/>
       <c r="C38" s="0"/>
-      <c r="G38" s="26"/>
+      <c r="G38" s="29"/>
       <c r="H38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="21" t="s">
-        <v>50</v>
+      <c r="A39" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="B39" s="0"/>
-      <c r="C39" s="11"/>
+      <c r="C39" s="13"/>
       <c r="G39" s="0"/>
-      <c r="H39" s="13" t="n">
+      <c r="H39" s="15" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="27" t="s">
-        <v>51</v>
+      <c r="A40" s="30" t="s">
+        <v>54</v>
       </c>
       <c r="B40" s="0"/>
       <c r="C40" s="0"/>
-      <c r="D40" s="28" t="n">
+      <c r="D40" s="31" t="n">
         <v>0.1</v>
       </c>
-      <c r="E40" s="29"/>
+      <c r="E40" s="32"/>
       <c r="F40" s="5"/>
       <c r="G40" s="0"/>
       <c r="H40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="27" t="s">
-        <v>52</v>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="30" t="s">
+        <v>55</v>
       </c>
       <c r="B41" s="0"/>
       <c r="C41" s="0"/>
-      <c r="D41" s="30" t="n">
-        <v>1.66666</v>
-      </c>
-      <c r="E41" s="31"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="34"/>
       <c r="F41" s="5"/>
       <c r="G41" s="0"/>
       <c r="H41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="27" t="s">
-        <v>53</v>
+      <c r="A42" s="30" t="s">
+        <v>56</v>
       </c>
       <c r="B42" s="0"/>
       <c r="C42" s="0"/>
-      <c r="D42" s="30" t="n">
+      <c r="D42" s="33" t="n">
         <v>-3.8</v>
       </c>
-      <c r="E42" s="31"/>
+      <c r="E42" s="34"/>
       <c r="F42" s="5"/>
       <c r="G42" s="0"/>
       <c r="H42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="27" t="s">
-        <v>54</v>
+      <c r="A43" s="30" t="s">
+        <v>57</v>
       </c>
       <c r="B43" s="0"/>
       <c r="C43" s="0"/>
-      <c r="D43" s="30" t="n">
+      <c r="D43" s="33" t="n">
         <v>7.1</v>
       </c>
-      <c r="E43" s="31"/>
-      <c r="F43" s="11"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="13"/>
       <c r="G43" s="0"/>
       <c r="H43" s="0"/>
     </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="27" t="s">
-        <v>55</v>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="30" t="s">
+        <v>58</v>
       </c>
       <c r="B44" s="0"/>
       <c r="C44" s="0"/>
-      <c r="D44" s="30" t="n">
+      <c r="D44" s="33" t="n">
         <v>90</v>
       </c>
-      <c r="E44" s="31"/>
-      <c r="F44" s="11"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="13"/>
       <c r="G44" s="0"/>
       <c r="H44" s="0"/>
     </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="27" t="s">
-        <v>56</v>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="B45" s="0"/>
       <c r="C45" s="0"/>
-      <c r="D45" s="32" t="n">
-        <v>989</v>
-      </c>
-      <c r="E45" s="33"/>
-      <c r="F45" s="11"/>
+      <c r="D45" s="35" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E45" s="36"/>
+      <c r="F45" s="13"/>
       <c r="G45" s="0"/>
       <c r="H45" s="0"/>
     </row>
@@ -1809,17 +1867,17 @@
       <c r="C46" s="0"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
-      <c r="F46" s="11"/>
+      <c r="F46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B47" s="0"/>
       <c r="C47" s="0"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="11"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="13"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
@@ -1827,22 +1885,22 @@
       <c r="C48" s="0"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
-      <c r="F48" s="11"/>
+      <c r="F48" s="13"/>
     </row>
     <row r="49" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" s="16"/>
+      <c r="A49" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="18"/>
       <c r="C49" s="7"/>
       <c r="E49" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="F49" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="F49" s="13"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B50" s="0"/>
       <c r="C50" s="0"/>
@@ -1850,52 +1908,52 @@
       <c r="E50" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="F50" s="11"/>
+      <c r="F50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="34"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="35"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B52" s="0"/>
       <c r="C52" s="0"/>
-      <c r="F52" s="36"/>
+      <c r="F52" s="39"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B53" s="0"/>
       <c r="C53" s="0"/>
-      <c r="F53" s="37"/>
+      <c r="F53" s="40"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B54" s="0"/>
       <c r="C54" s="0"/>
-      <c r="F54" s="38"/>
+      <c r="F54" s="41"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B55" s="0"/>
       <c r="C55" s="0"/>
-      <c r="F55" s="37"/>
+      <c r="F55" s="40"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B56" s="0"/>
       <c r="C56" s="0"/>
-      <c r="F56" s="24"/>
+      <c r="F56" s="27"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
@@ -1905,11 +1963,11 @@
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B58" s="0"/>
       <c r="C58" s="0"/>
-      <c r="E58" s="39"/>
+      <c r="E58" s="42"/>
       <c r="F58" s="5"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,11 +1975,11 @@
       <c r="C59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="27" t="s">
-        <v>67</v>
+      <c r="A60" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C60" s="5"/>
     </row>
@@ -1955,22 +2013,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="21.4030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="22.9744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="23.0459183673469"/>
-    <col collapsed="false" hidden="false" max="252" min="4" style="40" width="10.4132653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="43" width="21.4030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="43" width="22.9744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="23.0459183673469"/>
+    <col collapsed="false" hidden="false" max="252" min="4" style="43" width="10.4132653061225"/>
     <col collapsed="false" hidden="false" max="1025" min="253" style="0" width="10.4132653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
-      <c r="B1" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="42"/>
+      <c r="B1" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="45"/>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
@@ -2222,7 +2280,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>1</v>
@@ -2481,16 +2539,16 @@
       <c r="IR2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="43" t="n">
+      <c r="A3" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="46" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="43" t="n">
+      <c r="C3" s="46" t="n">
         <v>3.1436</v>
       </c>
-      <c r="D3" s="44"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="0"/>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
@@ -2741,13 +2799,13 @@
       <c r="IR3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="43" t="n">
+      <c r="A4" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="46" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="43" t="n">
+      <c r="C4" s="46" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="0"/>
@@ -3001,8 +3059,8 @@
       <c r="IR4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
-        <v>74</v>
+      <c r="A5" s="30" t="s">
+        <v>77</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>512</v>
@@ -3261,13 +3319,13 @@
       <c r="IR5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="43" t="n">
+      <c r="A6" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="46" t="n">
         <v>90</v>
       </c>
-      <c r="C6" s="43" t="n">
+      <c r="C6" s="46" t="n">
         <v>88.3</v>
       </c>
       <c r="D6" s="0"/>
@@ -3521,13 +3579,13 @@
       <c r="IR6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="43" t="n">
+      <c r="A7" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="46" t="n">
         <v>9</v>
       </c>
-      <c r="C7" s="43" t="n">
+      <c r="C7" s="46" t="n">
         <v>9</v>
       </c>
       <c r="D7" s="0"/>
@@ -3781,8 +3839,8 @@
       <c r="IR7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="s">
-        <v>77</v>
+      <c r="A8" s="30" t="s">
+        <v>80</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>1500</v>
@@ -4042,12 +4100,12 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="47" t="n">
+        <v>81</v>
+      </c>
+      <c r="B9" s="50" t="n">
         <v>100000000</v>
       </c>
-      <c r="C9" s="47" t="n">
+      <c r="C9" s="50" t="n">
         <v>100000000</v>
       </c>
       <c r="D9" s="0"/>
@@ -4302,12 +4360,12 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="47" t="n">
+        <v>82</v>
+      </c>
+      <c r="B10" s="50" t="n">
         <v>100000000</v>
       </c>
-      <c r="C10" s="47" t="n">
+      <c r="C10" s="50" t="n">
         <v>100000000</v>
       </c>
       <c r="D10" s="0"/>
@@ -4561,8 +4619,8 @@
       <c r="IR10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34" t="s">
-        <v>80</v>
+      <c r="A11" s="37" t="s">
+        <v>83</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0"/>
@@ -4818,9 +4876,9 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="48"/>
+        <v>84</v>
+      </c>
+      <c r="B12" s="51"/>
       <c r="C12" s="0"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
@@ -5074,7 +5132,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B13" s="0"/>
       <c r="C13" s="0"/>
@@ -5329,13 +5387,13 @@
       <c r="IR13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="50" t="n">
+      <c r="A14" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="53" t="n">
         <v>-1</v>
       </c>
-      <c r="C14" s="50" t="n">
+      <c r="C14" s="53" t="n">
         <v>2</v>
       </c>
       <c r="D14" s="0"/>
@@ -5589,11 +5647,11 @@
       <c r="IR14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="51" t="s">
-        <v>84</v>
+      <c r="A15" s="54" t="s">
+        <v>87</v>
       </c>
       <c r="B15" s="0"/>
-      <c r="C15" s="52"/>
+      <c r="C15" s="55"/>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
       <c r="F15" s="0"/>
@@ -5845,11 +5903,11 @@
       <c r="IR15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="51" t="s">
-        <v>85</v>
+      <c r="A16" s="54" t="s">
+        <v>88</v>
       </c>
       <c r="B16" s="0"/>
-      <c r="C16" s="52"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="0"/>
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
@@ -6101,11 +6159,11 @@
       <c r="IR16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
+      <c r="A17" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="57"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
       <c r="F17" s="0"/>
@@ -6358,7 +6416,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
@@ -6615,7 +6673,7 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
       <c r="B19" s="0"/>
-      <c r="C19" s="56"/>
+      <c r="C19" s="59"/>
       <c r="D19" s="0"/>
       <c r="E19" s="0"/>
       <c r="F19" s="0"/>
@@ -6868,10 +6926,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="56"/>
+        <v>91</v>
+      </c>
+      <c r="B20" s="51"/>
+      <c r="C20" s="59"/>
       <c r="D20" s="0"/>
       <c r="E20" s="0"/>
       <c r="F20" s="0"/>
@@ -7124,10 +7182,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="56"/>
+        <v>92</v>
+      </c>
+      <c r="B21" s="51"/>
+      <c r="C21" s="59"/>
       <c r="D21" s="0"/>
       <c r="E21" s="0"/>
       <c r="F21" s="0"/>
@@ -7380,7 +7438,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B22" s="0"/>
       <c r="C22" s="0"/>
@@ -7636,7 +7694,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
@@ -7892,7 +7950,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B24" s="0"/>
       <c r="C24" s="0"/>
@@ -8402,7 +8460,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>15</v>
@@ -8662,7 +8720,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>2</v>
@@ -8927,7 +8985,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>512</v>
@@ -8938,7 +8996,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>512</v>
@@ -8949,7 +9007,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -8960,7 +9018,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -8971,7 +9029,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B33" s="0"/>
       <c r="C33" s="0"/>
@@ -8983,23 +9041,23 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="57" t="n">
+        <v>103</v>
+      </c>
+      <c r="B35" s="60" t="n">
         <v>65.1186367</v>
       </c>
-      <c r="C35" s="57" t="n">
+      <c r="C35" s="60" t="n">
         <v>65.12657</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36" s="57" t="n">
+        <v>104</v>
+      </c>
+      <c r="B36" s="60" t="n">
         <v>-147.432975</v>
       </c>
-      <c r="C36" s="57" t="n">
+      <c r="C36" s="60" t="n">
         <v>-147.496908333</v>
       </c>
     </row>
@@ -9010,7 +9068,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B38" s="4" t="n">
         <v>77.51</v>
@@ -9021,7 +9079,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B39" s="4" t="n">
         <v>19.92</v>
@@ -9032,24 +9090,24 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -9087,44 +9145,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="58" t="n">
+        <v>123</v>
+      </c>
+      <c r="B2" s="61" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -9160,7 +9218,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>-1.5</v>
@@ -9198,19 +9256,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>0.5</v>
@@ -9248,7 +9306,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>1</v>
@@ -9286,83 +9344,83 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>5000</v>
@@ -9400,45 +9458,45 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="47" t="n">
+        <v>134</v>
+      </c>
+      <c r="B12" s="50" t="n">
         <v>2800000000000</v>
       </c>
-      <c r="C12" s="47" t="n">
+      <c r="C12" s="50" t="n">
         <v>2800000000000</v>
       </c>
-      <c r="D12" s="47" t="n">
+      <c r="D12" s="50" t="n">
         <v>2800000000000</v>
       </c>
-      <c r="E12" s="47" t="n">
+      <c r="E12" s="50" t="n">
         <v>2800000000000</v>
       </c>
-      <c r="F12" s="47" t="n">
+      <c r="F12" s="50" t="n">
         <v>2800000000000</v>
       </c>
-      <c r="G12" s="47" t="n">
+      <c r="G12" s="50" t="n">
         <v>2800000000000</v>
       </c>
-      <c r="H12" s="47" t="n">
+      <c r="H12" s="50" t="n">
         <v>2800000000000</v>
       </c>
-      <c r="I12" s="47" t="n">
+      <c r="I12" s="50" t="n">
         <v>2800000000000</v>
       </c>
-      <c r="J12" s="47" t="n">
+      <c r="J12" s="50" t="n">
         <v>2800000000000</v>
       </c>
-      <c r="K12" s="47" t="n">
+      <c r="K12" s="50" t="n">
         <v>2800000000000</v>
       </c>
-      <c r="L12" s="47" t="n">
+      <c r="L12" s="50" t="n">
         <v>2800000000000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.375</v>
@@ -9476,7 +9534,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.8</v>
@@ -9514,7 +9572,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>2.5</v>
@@ -9552,7 +9610,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>3.5</v>
@@ -9590,7 +9648,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>10000</v>
@@ -9628,7 +9686,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.2</v>

</xml_diff>